<commit_message>
Updated Standard Deviation code with absolute difference
</commit_message>
<xml_diff>
--- a/PTP_Isolation/Vel_10/Standard_Deviation and Max.xlsx
+++ b/PTP_Isolation/Vel_10/Standard_Deviation and Max.xlsx
@@ -460,22 +460,22 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>0.001754059062122603</v>
+        <v>0.001753054283238868</v>
       </c>
       <c r="C3" t="n">
-        <v>0.001056321054192696</v>
+        <v>0.001042925767129162</v>
       </c>
       <c r="D3" t="n">
-        <v>0.02414584786686625</v>
+        <v>0.008212652505215173</v>
       </c>
       <c r="E3" t="n">
-        <v>0.02059512765182459</v>
+        <v>0.01755742829292724</v>
       </c>
       <c r="F3" t="n">
-        <v>0.007395095671155635</v>
+        <v>0.007386946580121634</v>
       </c>
       <c r="G3" t="n">
-        <v>0.05787479087262525</v>
+        <v>0.04066989668766503</v>
       </c>
     </row>
     <row r="4">
@@ -485,7 +485,7 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>5.076092725614378e-05</v>
+        <v>0.005324698759889668</v>
       </c>
       <c r="C4" t="n">
         <v>0.003810255156690756</v>

</xml_diff>